<commit_message>
added header and interactive menu
</commit_message>
<xml_diff>
--- a/backend/bookings.xlsx
+++ b/backend/bookings.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -70,7 +70,7 @@
     <t>2026-02-04T09:38:56.432Z</t>
   </si>
   <si>
-    <t>confirmed</t>
+    <t>deleted</t>
   </si>
   <si>
     <t>admin-1770197953755-sdd19wp72</t>
@@ -97,9 +97,6 @@
     <t>2026-02-04T09:39:13.755Z</t>
   </si>
   <si>
-    <t>deleted</t>
-  </si>
-  <si>
     <t>admin-1770197989073-ln4belhx8</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>2026-02-04T09:39:49.073Z</t>
   </si>
   <si>
-    <t>active</t>
-  </si>
-  <si>
     <t>admin-1770197993632-ituym43kl</t>
   </si>
   <si>
@@ -143,6 +137,111 @@
   </si>
   <si>
     <t>2026-02-04T09:40:10.091Z</t>
+  </si>
+  <si>
+    <t>user-1770217230570-q16lgw2m4</t>
+  </si>
+  <si>
+    <t>small-6</t>
+  </si>
+  <si>
+    <t>2026-02-18</t>
+  </si>
+  <si>
+    <t>2026-02-04T15:00:30.570Z</t>
+  </si>
+  <si>
+    <t>user-1770269557423-v2mwc2mvr</t>
+  </si>
+  <si>
+    <t>2026-02-13</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2026-02-05T05:32:37.423Z</t>
+  </si>
+  <si>
+    <t>user-1770269654810-hdcfop7z8</t>
+  </si>
+  <si>
+    <t>2026-02-12</t>
+  </si>
+  <si>
+    <t>2026-02-21</t>
+  </si>
+  <si>
+    <t>2026-02-05T05:34:14.810Z</t>
+  </si>
+  <si>
+    <t>user-1770269695556-crjmq8by7</t>
+  </si>
+  <si>
+    <t>2026-06-17</t>
+  </si>
+  <si>
+    <t>2026-06-26</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2026-02-05T05:34:55.556Z</t>
+  </si>
+  <si>
+    <t>user-1770269764219-oasf7qz8t</t>
+  </si>
+  <si>
+    <t>2026-02-05T05:36:04.219Z</t>
+  </si>
+  <si>
+    <t>user-1770269799451-h8rgp2qs2</t>
+  </si>
+  <si>
+    <t>2026-02-11</t>
+  </si>
+  <si>
+    <t>2026-02-19</t>
+  </si>
+  <si>
+    <t>2026-02-05T05:36:39.452Z</t>
+  </si>
+  <si>
+    <t>user-1770271881756-s55d3ixyi</t>
+  </si>
+  <si>
+    <t>2026-02-05T06:11:21.756Z</t>
+  </si>
+  <si>
+    <t>user-1770272164903-jnrqyxl8l</t>
+  </si>
+  <si>
+    <t>2026-02-05T06:16:04.903Z</t>
+  </si>
+  <si>
+    <t>user-1770272369480-z84bsit6g</t>
+  </si>
+  <si>
+    <t>2026-02-10</t>
+  </si>
+  <si>
+    <t>+79015545015</t>
+  </si>
+  <si>
+    <t>2026-02-05T06:19:29.480Z</t>
+  </si>
+  <si>
+    <t>user-1770284364545-x5swu67fa</t>
+  </si>
+  <si>
+    <t>2026-02-05T09:39:24.545Z</t>
+  </si>
+  <si>
+    <t>user-1770285718054-dnm83l4fy</t>
+  </si>
+  <si>
+    <t>2026-02-05T10:01:58.054Z</t>
   </si>
 </sst>
 </file>
@@ -161,7 +260,7 @@
       <b/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,11 +270,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE0E0E0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -196,13 +290,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -544,7 +635,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J18"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -621,52 +712,52 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>28</v>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>25</v>
@@ -678,15 +769,15 @@
         <v>26</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -698,7 +789,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>25</v>
@@ -710,27 +801,27 @@
         <v>26</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>25</v>
@@ -742,41 +833,393 @@
         <v>26</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added price for entire stay
</commit_message>
<xml_diff>
--- a/backend/bookings.xlsx
+++ b/backend/bookings.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -242,6 +242,33 @@
   </si>
   <si>
     <t>2026-02-05T10:01:58.054Z</t>
+  </si>
+  <si>
+    <t>user-1770292489867-t9l1zdx3p</t>
+  </si>
+  <si>
+    <t>small-1</t>
+  </si>
+  <si>
+    <t>2026-04-06</t>
+  </si>
+  <si>
+    <t>2026-04-10</t>
+  </si>
+  <si>
+    <t>+87776665544</t>
+  </si>
+  <si>
+    <t>2026-02-05T11:54:49.867Z</t>
+  </si>
+  <si>
+    <t>confirmed</t>
+  </si>
+  <si>
+    <t>user-1770292553493-693dbwhkl</t>
+  </si>
+  <si>
+    <t>2026-02-05T11:55:53.493Z</t>
   </si>
 </sst>
 </file>
@@ -260,7 +287,7 @@
       <b/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +304,11 @@
         <fgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -290,10 +322,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -635,7 +670,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -1223,6 +1258,70 @@
         <v>19</v>
       </c>
     </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>